<commit_message>
track files created/used to ease reproduction
</commit_message>
<xml_diff>
--- a/global_river_mining_where_figs_are_in_code.xlsx
+++ b/global_river_mining_where_figs_are_in_code.xlsx
@@ -8,24 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bowdoin-my.sharepoint.com/personal/e_dethier_bowdoin_edu/Documents/research/global-alluvial-mining/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="144" documentId="8_{39B3B084-0981-644E-824D-75D994C37022}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BCFDA8DE-BAA9-C14A-A9AA-323E1B94ACFD}"/>
+  <xr:revisionPtr revIDLastSave="168" documentId="8_{39B3B084-0981-644E-824D-75D994C37022}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{14014CFD-BACB-5549-BFBD-37E4074E7BAB}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{1AFEF7FB-17E6-7E40-B3A2-C4624379F8C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="95">
   <si>
     <t>Fig 1</t>
   </si>
@@ -240,12 +251,6 @@
     <t xml:space="preserve">Quantification of mining area and small river length affected by river mineral mining. </t>
   </si>
   <si>
-    <t>Need to add a,b,c</t>
-  </si>
-  <si>
-    <t>Need to add a,b</t>
-  </si>
-  <si>
     <t xml:space="preserve">Reference (pre-mining) and active-mining suspended sediment concentration (SSC) histograms for some analyzed rivers in Africa. </t>
   </si>
   <si>
@@ -310,6 +315,12 @@
   </si>
   <si>
     <t>2.12A</t>
+  </si>
+  <si>
+    <t>3.4</t>
+  </si>
+  <si>
+    <t>4.2</t>
   </si>
 </sst>
 </file>
@@ -377,7 +388,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -392,6 +403,26 @@
       </right>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -413,7 +444,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -427,9 +458,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -744,10 +777,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{803FB51A-44E6-FD4C-AE10-7767D54FAF92}">
-  <dimension ref="A1:K37"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -759,7 +792,7 @@
     <col min="10" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>20</v>
       </c>
@@ -791,657 +824,654 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C2" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C3" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C4" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C5" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>33</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" s="7" t="s">
+      <c r="C6" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="11" t="s">
         <v>17</v>
       </c>
       <c r="J6" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>34</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
+      <c r="C7" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
       <c r="J7" s="7"/>
     </row>
-    <row r="8" spans="1:11" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>35</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
+      <c r="C8" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
       <c r="J8" s="7"/>
     </row>
-    <row r="9" spans="1:11" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>36</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
+      <c r="C9" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
       <c r="J9" s="7"/>
     </row>
-    <row r="10" spans="1:11" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>37</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C10" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
+      <c r="C10" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
       <c r="J10" s="7"/>
     </row>
-    <row r="11" spans="1:11" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>38</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
+      <c r="C11" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
       <c r="J11" s="7"/>
     </row>
-    <row r="12" spans="1:11" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>39</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
+      <c r="C12" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
       <c r="J12" s="7"/>
-      <c r="K12" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:10" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>40</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C13" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
+      <c r="C13" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
       <c r="J13" s="7"/>
     </row>
-    <row r="14" spans="1:11" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>41</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
+      <c r="C14" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
       <c r="J14" s="7"/>
     </row>
-    <row r="15" spans="1:11" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C15" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
+      <c r="C15" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
       <c r="J15" s="7"/>
-      <c r="K15" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:10" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="C16" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
+      <c r="C16" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
       <c r="J16" s="7"/>
     </row>
-    <row r="17" spans="1:11" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="C17" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
+      <c r="C17" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
       <c r="J17" s="7"/>
     </row>
-    <row r="18" spans="1:11" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
+      <c r="C18" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
       <c r="J18" s="7"/>
     </row>
-    <row r="19" spans="1:11" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C19" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
+      <c r="C19" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
       <c r="J19" s="7"/>
     </row>
-    <row r="20" spans="1:11" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="C20" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
+      <c r="C20" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
       <c r="J20" s="7"/>
     </row>
-    <row r="21" spans="1:11" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="C21" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
+      <c r="C21" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
       <c r="J21" s="7"/>
-      <c r="K21" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:10" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="C22" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
+      <c r="C22" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
       <c r="J22" s="7"/>
     </row>
-    <row r="23" spans="1:11" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="C23" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
+      <c r="C23" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
       <c r="J23" s="7"/>
     </row>
-    <row r="24" spans="1:11" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C24" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
+      <c r="C24" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
       <c r="J24" s="7"/>
     </row>
-    <row r="25" spans="1:11" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
+      <c r="C25" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
       <c r="J25" s="7"/>
-      <c r="K25" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:10" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
+        <v>71</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
       <c r="J26" s="7"/>
     </row>
-    <row r="27" spans="1:11" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
+        <v>72</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
       <c r="J27" s="7"/>
     </row>
-    <row r="28" spans="1:11" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
+        <v>73</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
       <c r="J28" s="7"/>
     </row>
-    <row r="29" spans="1:11" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
         <v>44</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
-      <c r="I29" s="7"/>
+        <v>74</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
       <c r="J29" s="7"/>
-      <c r="K29" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:10" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
         <v>45</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
+        <v>75</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
       <c r="J30" s="7"/>
     </row>
-    <row r="31" spans="1:11" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
         <v>46</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
+        <v>76</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
       <c r="J31" s="7"/>
     </row>
-    <row r="32" spans="1:11" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
         <v>47</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="7"/>
+        <v>77</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="11"/>
       <c r="J32" s="7"/>
     </row>
     <row r="33" spans="1:10" ht="35" customHeight="1" x14ac:dyDescent="0.2">
@@ -1449,17 +1479,17 @@
         <v>48</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="C33" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="7"/>
+        <v>78</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="11"/>
       <c r="J33" s="7"/>
     </row>
     <row r="34" spans="1:10" ht="35" customHeight="1" x14ac:dyDescent="0.2">
@@ -1467,19 +1497,19 @@
         <v>49</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="7"/>
-      <c r="I34" s="7"/>
+        <v>79</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="11"/>
       <c r="J34" s="7"/>
     </row>
     <row r="35" spans="1:10" ht="35" customHeight="1" x14ac:dyDescent="0.2">
@@ -1487,19 +1517,19 @@
         <v>50</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="7"/>
-      <c r="H35" s="7"/>
-      <c r="I35" s="7"/>
+        <v>80</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="11"/>
       <c r="J35" s="7"/>
     </row>
     <row r="36" spans="1:10" ht="35" customHeight="1" x14ac:dyDescent="0.2">
@@ -1507,20 +1537,20 @@
         <v>51</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7"/>
-      <c r="G36" s="7"/>
-      <c r="H36" s="7"/>
-      <c r="I36" s="7"/>
-      <c r="J36" s="7"/>
+        <v>81</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
+      <c r="I36" s="8"/>
+      <c r="J36" s="9"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="6"/>

</xml_diff>